<commit_message>
update grafik di excel
</commit_message>
<xml_diff>
--- a/literatur/bab4/pengujian/Book1.xlsx
+++ b/literatur/bab4/pengujian/Book1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\banca\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IPeKa35\tea-bg\literatur\bab4\pengujian\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D066929B-37D4-4D0B-B927-50E9BBA85868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69FA626F-2FDA-43BA-A257-4C0DADF5CD00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{6D566884-366D-4A70-A22F-7784A8BE6070}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6D566884-366D-4A70-A22F-7784A8BE6070}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1723,7 +1723,7 @@
                       </a:sysClr>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t>Durasi Waktu Peningkatan Kelembaban (%)</a:t>
+                  <a:t>Durasi Waktu Peningkatan Kelembaban (d)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2277,7 +2277,7 @@
                       </a:sysClr>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t>Durasi Waktu Penurunan Kelembaban (%)</a:t>
+                  <a:t>Durasi Waktu Penurunan Kelembaban (d)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -5025,8 +5025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0552165B-EC40-44BD-AD23-51CCD24E8C67}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView zoomScale="82" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B6" zoomScale="71" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5380,7 +5380,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EC2AD52-1980-42F1-B9F4-940CC402470F}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>